<commit_message>
add counter for existing file
</commit_message>
<xml_diff>
--- a/DownloadFolderManager/rules.xlsx
+++ b/DownloadFolderManager/rules.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Work and projects\App&amp;Utils\DownloadFolderManager\Worker.DownloadFolderManager\DownloadFolderManager\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="24915" windowHeight="12600" activeTab="1"/>
   </bookViews>
@@ -22,7 +27,7 @@
     <author>Deny</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -183,15 +188,9 @@
     <t>doc-vodnestocne</t>
   </si>
   <si>
-    <t>*.docx</t>
-  </si>
-  <si>
     <t>Vodné a stočné</t>
   </si>
   <si>
-    <t>M:\Document\Documents\Invoice\Paid\Watter</t>
-  </si>
-  <si>
     <t>Serials youngsheldon 3</t>
   </si>
   <si>
@@ -204,32 +203,41 @@
     <t>F:\Serials\_Unknow</t>
   </si>
   <si>
-    <t>F:\Filmy</t>
-  </si>
-  <si>
     <t>D:\Downloads\Documents</t>
   </si>
   <si>
     <t>doc-vyplatni paska</t>
   </si>
   <si>
-    <t>*.pdf</t>
-  </si>
-  <si>
     <t>826_Michna_\d{4}_\d{2}</t>
   </si>
   <si>
-    <t>M:\Document\Payslip</t>
-  </si>
-  <si>
     <t>\\denynaspc\Filmy\Serials\Young sheldon\03</t>
+  </si>
+  <si>
+    <t>\\denynaspc\Serials\_Unknow</t>
+  </si>
+  <si>
+    <t>\\denynaspc\Filmy\Filmy</t>
+  </si>
+  <si>
+    <t>\\denynaspc\Me\Document\Payslip</t>
+  </si>
+  <si>
+    <t>.pdf</t>
+  </si>
+  <si>
+    <t>.docx</t>
+  </si>
+  <si>
+    <t>\\denynaspc\Me\Document\Documents\Invoice\Paid\Watter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +267,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -277,14 +294,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -293,12 +313,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -340,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +398,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,7 +638,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,30 +669,30 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -682,8 +705,8 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>49</v>
+      <c r="E4" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,8 +730,8 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>50</v>
+      <c r="E6" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -719,7 +742,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,16 +819,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,13 +836,13 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,12 +853,16 @@
         <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E6" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>